<commit_message>
feat: Establish core application infrastructure including API, UI components, Supabase integration, and initial data/requirements.
</commit_message>
<xml_diff>
--- a/0. Dati Iniziali/PortfolioMP_Acquisti.xlsx
+++ b/0. Dati Iniziali/PortfolioMP_Acquisti.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\PerixMonitor\0. Dati Iniziali\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F088CCA2-CA94-4D06-A3D0-0D40B9AA3E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F31061E-3A9E-4A9A-8DDB-A5C841F3B77E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="490" windowWidth="38620" windowHeight="21220" xr2:uid="{461EA0C3-CC98-4DCD-BC5C-C997A9959903}"/>
   </bookViews>
@@ -288,7 +288,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -309,12 +309,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -383,11 +389,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="9"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="9"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -425,45 +446,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="8" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="21">
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -533,6 +532,36 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -815,10 +844,10 @@
     <tableColumn id="8" xr3:uid="{8C52C664-8EA8-4E89-892F-C9CCC6BB2E54}" name="Prezzo Operazione (EUR)" dataDxfId="10">
       <calculatedColumnFormula>+Table1[[#This Row],[Prezzo Carico (EUR)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{20AB3F10-3CEF-4BB7-ACA8-F58F613D5EBF}" name="Prezzo Corrente (EUR)" dataDxfId="1">
+    <tableColumn id="9" xr3:uid="{20AB3F10-3CEF-4BB7-ACA8-F58F613D5EBF}" name="Prezzo Corrente (EUR)" dataDxfId="9">
       <calculatedColumnFormula>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{7F8241B6-2FCB-4564-8F24-4D4146A82E8B}" name="Controvalore (EUR)" dataDxfId="0">
+    <tableColumn id="10" xr3:uid="{7F8241B6-2FCB-4564-8F24-4D4146A82E8B}" name="Controvalore (EUR)" dataDxfId="8">
       <calculatedColumnFormula>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1143,10 +1172,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{840B4B52-5CB9-41B5-89C1-B1D0A0795C06}">
-  <dimension ref="A1:Q23"/>
+  <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1161,10 +1190,12 @@
     <col min="8" max="8" width="23.08984375" customWidth="1"/>
     <col min="9" max="9" width="21.90625" customWidth="1"/>
     <col min="10" max="10" width="24.54296875" customWidth="1"/>
-    <col min="15" max="15" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.7265625" customWidth="1"/>
+    <col min="16" max="16" width="13.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1196,7 +1227,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>11</v>
       </c>
@@ -1231,7 +1262,7 @@
         <v>18262.960000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>12</v>
       </c>
@@ -1265,8 +1296,14 @@
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>22595</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="N3" s="21">
+        <v>-22708.055199999999</v>
+      </c>
+      <c r="O3" s="23">
+        <v>45355</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>13</v>
       </c>
@@ -1300,8 +1337,27 @@
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>22708.055199999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="M4" s="4">
+        <v>32.729999999999997</v>
+      </c>
+      <c r="N4" s="4">
+        <f>+C4*M4</f>
+        <v>25735.271699999998</v>
+      </c>
+      <c r="O4" s="22">
+        <f ca="1">TODAY()</f>
+        <v>46048</v>
+      </c>
+      <c r="P4" s="4">
+        <f>+N4-J4</f>
+        <v>3027.2164999999986</v>
+      </c>
+      <c r="R4" s="24">
+        <f ca="1">XIRR(N3:N4,O3:O4)</f>
+        <v>6.8132868409156805E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>14</v>
       </c>
@@ -1336,7 +1392,7 @@
         <v>94906.594379999995</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>15</v>
       </c>
@@ -1371,7 +1427,7 @@
         <v>61941.047500000001</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
         <v>16</v>
       </c>
@@ -1406,7 +1462,7 @@
         <v>5026.6897799999997</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>17</v>
       </c>
@@ -1441,7 +1497,7 @@
         <v>5080.5599869999996</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>18</v>
       </c>
@@ -1476,7 +1532,7 @@
         <v>15989.990029199998</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
         <v>19</v>
       </c>
@@ -1511,7 +1567,7 @@
         <v>15990</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
         <v>20</v>
       </c>
@@ -1546,7 +1602,7 @@
         <v>20766.498900000002</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>21</v>
       </c>
@@ -1581,7 +1637,7 @@
         <v>24528.056350000003</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>22</v>
       </c>
@@ -1616,7 +1672,7 @@
         <v>14342.336184</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
         <v>23</v>
       </c>
@@ -1651,7 +1707,7 @@
         <v>22232.444</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
         <v>24</v>
       </c>
@@ -1686,7 +1742,7 @@
         <v>24352.845929999999</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
         <v>25</v>
       </c>
@@ -1721,7 +1777,7 @@
         <v>11192.982</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
         <v>26</v>
       </c>
@@ -1756,7 +1812,7 @@
         <v>8014.7699999999995</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
         <v>27</v>
       </c>
@@ -1791,7 +1847,7 @@
         <v>9985</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
         <v>28</v>
       </c>
@@ -1826,7 +1882,7 @@
         <v>19428</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20" s="14" t="s">
         <v>52</v>
       </c>
@@ -1861,9 +1917,9 @@
         <v>14666.299950000001</v>
       </c>
       <c r="M20" s="1"/>
-      <c r="Q20" s="1"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R20" s="1"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A21" s="14" t="s">
         <v>53</v>
       </c>
@@ -1898,7 +1954,7 @@
         <v>101163.77879299999</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
         <v>54</v>
       </c>
@@ -1933,9 +1989,9 @@
         <v>15141.96999</v>
       </c>
       <c r="M22" s="1"/>
-      <c r="Q22" s="1"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="R22" s="1"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A23" s="14" t="s">
         <v>55</v>
       </c>
@@ -1970,35 +2026,35 @@
         <v>19889.499954999999</v>
       </c>
       <c r="M23" s="1"/>
-      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A23">
-    <cfRule type="containsText" dxfId="9" priority="16" stopIfTrue="1" operator="containsText" text="BTP">
+    <cfRule type="containsText" dxfId="7" priority="16" stopIfTrue="1" operator="containsText" text="BTP">
       <formula>NOT(ISERROR(SEARCH("BTP",A2)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="17" stopIfTrue="1">
       <formula>IF(AND(ISNUMBER(SEARCH("H2O", A2)), ISNUMBER(SEARCH("SP", A2))), 1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C23">
-    <cfRule type="containsBlanks" dxfId="7" priority="14">
+    <cfRule type="containsBlanks" dxfId="5" priority="14">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D23">
-    <cfRule type="notContainsText" dxfId="6" priority="18" stopIfTrue="1" operator="notContains" text="EUR">
+    <cfRule type="notContainsText" dxfId="4" priority="18" stopIfTrue="1" operator="notContains" text="EUR">
       <formula>ISERROR(SEARCH("EUR",D2))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="5" priority="18">
+    <cfRule type="containsBlanks" dxfId="3" priority="18">
       <formula>LEN(TRIM(D2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G23">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="Vendita">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Vendita">
       <formula>NOT(ISERROR(SEARCH("Vendita",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="Acquisto">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Acquisto">
       <formula>NOT(ISERROR(SEARCH("Acquisto",G2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
20260127 Tipo Asset e Liquidità
</commit_message>
<xml_diff>
--- a/0. Dati Iniziali/PortfolioMP_Acquisti.xlsx
+++ b/0. Dati Iniziali/PortfolioMP_Acquisti.xlsx
@@ -2,20 +2,20 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\PerixMonitor\0. Dati Iniziali\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F31061E-3A9E-4A9A-8DDB-A5C841F3B77E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6FC9E3-1146-40EF-AB33-217849B2528A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="490" windowWidth="38620" windowHeight="21220" xr2:uid="{461EA0C3-CC98-4DCD-BC5C-C997A9959903}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcMode="manual"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="65">
   <si>
     <t>Descrizione Titolo</t>
   </si>
@@ -241,6 +241,30 @@
   </si>
   <si>
     <t>Controvalore (EUR)</t>
+  </si>
+  <si>
+    <t>Fondo Obblig. Governativo</t>
+  </si>
+  <si>
+    <t>Fondo Azionario</t>
+  </si>
+  <si>
+    <t>Multi-Asset</t>
+  </si>
+  <si>
+    <t>ETF azionario</t>
+  </si>
+  <si>
+    <t>Fondo Obbligazionario</t>
+  </si>
+  <si>
+    <t>Tipologia</t>
+  </si>
+  <si>
+    <t>Certificato</t>
+  </si>
+  <si>
+    <t>Altro</t>
   </si>
 </sst>
 </file>
@@ -449,20 +473,41 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="8" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="37">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -473,14 +518,107 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FFEB8953"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.89996032593768116"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFEB8953"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -523,6 +661,36 @@
           <bgColor theme="7" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <color auto="1"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <fill>
+        <patternFill patternType="gray0625">
+          <fgColor theme="9" tint="0.79998168889431442"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
@@ -831,23 +999,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{04F4BF02-F5A0-427F-92C4-A60283CF04F1}" name="Table1" displayName="Table1" ref="A1:J23" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19" tableBorderDxfId="18">
-  <autoFilter ref="A1:J23" xr:uid="{04F4BF02-F5A0-427F-92C4-A60283CF04F1}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{B8061C36-8993-4203-ABD6-C7BF7558D40C}" name="Descrizione Titolo" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{C4CDF0AD-2602-44A7-AA26-292542A274A0}" name="ISIN" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{0A18EC50-C250-41F4-83C1-E84B3FDD76A5}" name="Quantità" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{F21CA34D-52E3-4C7A-A959-24C01F694687}" name="Divisa" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{5C9AD5B2-888B-43C8-AC2C-1789ADAB0AD8}" name="Prezzo Carico (EUR)" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{1CC3BD49-EF04-4684-84DC-5AB42F08A1CD}" name="Data (acquisto/vendita)" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{0B72A75D-196B-42C0-9E49-163198DF8CDB}" name="Operazione" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{8C52C664-8EA8-4E89-892F-C9CCC6BB2E54}" name="Prezzo Operazione (EUR)" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{04F4BF02-F5A0-427F-92C4-A60283CF04F1}" name="Table1" displayName="Table1" ref="A1:K23" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35" tableBorderDxfId="34">
+  <autoFilter ref="A1:K23" xr:uid="{04F4BF02-F5A0-427F-92C4-A60283CF04F1}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{B8061C36-8993-4203-ABD6-C7BF7558D40C}" name="Descrizione Titolo" dataDxfId="33"/>
+    <tableColumn id="2" xr3:uid="{C4CDF0AD-2602-44A7-AA26-292542A274A0}" name="ISIN" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{0A18EC50-C250-41F4-83C1-E84B3FDD76A5}" name="Quantità" dataDxfId="31"/>
+    <tableColumn id="4" xr3:uid="{F21CA34D-52E3-4C7A-A959-24C01F694687}" name="Divisa" dataDxfId="30"/>
+    <tableColumn id="5" xr3:uid="{5C9AD5B2-888B-43C8-AC2C-1789ADAB0AD8}" name="Prezzo Carico (EUR)" dataDxfId="29"/>
+    <tableColumn id="6" xr3:uid="{1CC3BD49-EF04-4684-84DC-5AB42F08A1CD}" name="Data (acquisto/vendita)" dataDxfId="28"/>
+    <tableColumn id="7" xr3:uid="{0B72A75D-196B-42C0-9E49-163198DF8CDB}" name="Operazione" dataDxfId="27"/>
+    <tableColumn id="8" xr3:uid="{8C52C664-8EA8-4E89-892F-C9CCC6BB2E54}" name="Prezzo Operazione (EUR)" dataDxfId="26">
       <calculatedColumnFormula>+Table1[[#This Row],[Prezzo Carico (EUR)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{20AB3F10-3CEF-4BB7-ACA8-F58F613D5EBF}" name="Prezzo Corrente (EUR)" dataDxfId="9">
+    <tableColumn id="9" xr3:uid="{20AB3F10-3CEF-4BB7-ACA8-F58F613D5EBF}" name="Prezzo Corrente (EUR)" dataDxfId="25">
       <calculatedColumnFormula>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{7F8241B6-2FCB-4564-8F24-4D4146A82E8B}" name="Controvalore (EUR)" dataDxfId="8">
+    <tableColumn id="11" xr3:uid="{8B0704F8-8C2E-42BE-A30C-03EF7C2730A1}" name="Tipologia" dataDxfId="23"/>
+    <tableColumn id="10" xr3:uid="{7F8241B6-2FCB-4564-8F24-4D4146A82E8B}" name="Controvalore (EUR)" dataDxfId="24">
       <calculatedColumnFormula>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1172,10 +1341,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{840B4B52-5CB9-41B5-89C1-B1D0A0795C06}">
-  <dimension ref="A1:R23"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1190,12 +1360,15 @@
     <col min="8" max="8" width="23.08984375" customWidth="1"/>
     <col min="9" max="9" width="21.90625" customWidth="1"/>
     <col min="10" max="10" width="24.54296875" customWidth="1"/>
-    <col min="14" max="14" width="10.7265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.7265625" customWidth="1"/>
-    <col min="16" max="16" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1223,11 +1396,14 @@
       <c r="I1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="J1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="19" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>11</v>
       </c>
@@ -1257,12 +1433,15 @@
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>91.314800000000005</v>
       </c>
-      <c r="J2" s="20">
+      <c r="J2" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" s="20">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>18262.960000000003</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A3" s="10" t="s">
         <v>12</v>
       </c>
@@ -1292,18 +1471,21 @@
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>90.38</v>
       </c>
-      <c r="J3" s="20">
+      <c r="J3" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="K3" s="20">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>22595</v>
       </c>
-      <c r="N3" s="21">
+      <c r="O3" s="21">
         <v>-22708.055199999999</v>
       </c>
-      <c r="O3" s="23">
+      <c r="P3" s="22">
         <v>45355</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
         <v>13</v>
       </c>
@@ -1333,31 +1515,34 @@
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>28.88</v>
       </c>
-      <c r="J4" s="20">
+      <c r="J4" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="K4" s="20">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>22708.055199999999</v>
       </c>
-      <c r="M4" s="4">
+      <c r="N4" s="4">
         <v>32.729999999999997</v>
       </c>
-      <c r="N4" s="4">
-        <f>+C4*M4</f>
+      <c r="O4" s="4">
+        <f>+C4*N4</f>
         <v>25735.271699999998</v>
       </c>
-      <c r="O4" s="22">
+      <c r="P4" s="12">
         <f ca="1">TODAY()</f>
-        <v>46048</v>
-      </c>
-      <c r="P4" s="4">
-        <f>+N4-J4</f>
+        <v>46049</v>
+      </c>
+      <c r="Q4" s="4">
+        <f>+O4-K4</f>
         <v>3027.2164999999986</v>
       </c>
-      <c r="R4" s="24">
-        <f ca="1">XIRR(N3:N4,O3:O4)</f>
-        <v>6.8132868409156805E-2</v>
+      <c r="S4" s="23">
+        <f ca="1">XIRR(O3:O4,P3:P4)</f>
+        <v>6.8031427264213559E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" s="10" t="s">
         <v>14</v>
       </c>
@@ -1387,12 +1572,15 @@
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>117.33</v>
       </c>
-      <c r="J5" s="20">
+      <c r="J5" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="K5" s="20">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>94906.594379999995</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" s="10" t="s">
         <v>15</v>
       </c>
@@ -1422,12 +1610,15 @@
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>242.5</v>
       </c>
-      <c r="J6" s="20">
+      <c r="J6" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="K6" s="20">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>61941.047500000001</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="10" t="s">
         <v>16</v>
       </c>
@@ -1457,12 +1648,15 @@
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>8.8187540000000002</v>
       </c>
-      <c r="J7" s="20">
+      <c r="J7" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="K7" s="20">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>5026.6897799999997</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A8" s="10" t="s">
         <v>17</v>
       </c>
@@ -1492,12 +1686,15 @@
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>108.097021</v>
       </c>
-      <c r="J8" s="20">
+      <c r="J8" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="K8" s="20">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>5080.5599869999996</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A9" s="10" t="s">
         <v>18</v>
       </c>
@@ -1527,12 +1724,15 @@
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>16.910799999999998</v>
       </c>
-      <c r="J9" s="20">
+      <c r="J9" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="K9" s="20">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>15989.990029199998</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
         <v>19</v>
       </c>
@@ -1562,12 +1762,15 @@
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>5</v>
       </c>
-      <c r="J10" s="20">
+      <c r="J10" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="K10" s="20">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>15990</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="10" t="s">
         <v>20</v>
       </c>
@@ -1597,12 +1800,15 @@
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>198.97</v>
       </c>
-      <c r="J11" s="20">
+      <c r="J11" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="K11" s="20">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>20766.498900000002</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A12" s="10" t="s">
         <v>21</v>
       </c>
@@ -1632,12 +1838,15 @@
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>117.95</v>
       </c>
-      <c r="J12" s="20">
+      <c r="J12" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="K12" s="20">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>24528.056350000003</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A13" s="10" t="s">
         <v>22</v>
       </c>
@@ -1667,12 +1876,15 @@
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>32.000999999999998</v>
       </c>
-      <c r="J13" s="20">
+      <c r="J13" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="K13" s="20">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>14342.336184</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A14" s="10" t="s">
         <v>23</v>
       </c>
@@ -1702,12 +1914,15 @@
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>188.5</v>
       </c>
-      <c r="J14" s="20">
+      <c r="J14" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="K14" s="20">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>22232.444</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" s="10" t="s">
         <v>24</v>
       </c>
@@ -1737,12 +1952,15 @@
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>83.850999999999999</v>
       </c>
-      <c r="J15" s="20">
+      <c r="J15" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="K15" s="20">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>24352.845929999999</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" s="10" t="s">
         <v>25</v>
       </c>
@@ -1772,12 +1990,15 @@
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>19.100000000000001</v>
       </c>
-      <c r="J16" s="20">
+      <c r="J16" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="K16" s="20">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>11192.982</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
         <v>26</v>
       </c>
@@ -1807,12 +2028,15 @@
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>93.194999999999993</v>
       </c>
-      <c r="J17" s="20">
+      <c r="J17" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="K17" s="20">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>8014.7699999999995</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
         <v>27</v>
       </c>
@@ -1842,12 +2066,15 @@
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>100</v>
       </c>
-      <c r="J18" s="20">
+      <c r="J18" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="K18" s="20">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>9985</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
         <v>28</v>
       </c>
@@ -1877,12 +2104,15 @@
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>97.14</v>
       </c>
-      <c r="J19" s="20">
+      <c r="J19" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="K19" s="20">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>19428</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="14" t="s">
         <v>52</v>
       </c>
@@ -1912,14 +2142,16 @@
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>94.621290000000002</v>
       </c>
-      <c r="J20" s="20">
+      <c r="J20" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="K20" s="20">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>14666.299950000001</v>
       </c>
-      <c r="M20" s="1"/>
-      <c r="R20" s="1"/>
+      <c r="O20" s="1"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="14" t="s">
         <v>53</v>
       </c>
@@ -1949,12 +2181,15 @@
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>42.381138999999997</v>
       </c>
-      <c r="J21" s="20">
+      <c r="J21" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="K21" s="20">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>101163.77879299999</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" s="10" t="s">
         <v>54</v>
       </c>
@@ -1984,14 +2219,16 @@
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>1009.464666</v>
       </c>
-      <c r="J22" s="20">
+      <c r="J22" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="K22" s="20">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>15141.96999</v>
       </c>
-      <c r="M22" s="1"/>
-      <c r="R22" s="1"/>
+      <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="14" t="s">
         <v>55</v>
       </c>
@@ -2021,44 +2258,78 @@
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>97.021951000000001</v>
       </c>
-      <c r="J23" s="20">
+      <c r="J23" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="K23" s="20">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>19889.499954999999</v>
       </c>
-      <c r="M23" s="1"/>
-      <c r="R23" s="1"/>
+      <c r="O23" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A23">
-    <cfRule type="containsText" dxfId="7" priority="16" stopIfTrue="1" operator="containsText" text="BTP">
+    <cfRule type="containsText" dxfId="22" priority="32" stopIfTrue="1" operator="containsText" text="BTP">
       <formula>NOT(ISERROR(SEARCH("BTP",A2)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="33" stopIfTrue="1">
       <formula>IF(AND(ISNUMBER(SEARCH("H2O", A2)), ISNUMBER(SEARCH("SP", A2))), 1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C23">
-    <cfRule type="containsBlanks" dxfId="5" priority="14">
+    <cfRule type="containsBlanks" dxfId="20" priority="30">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D23">
-    <cfRule type="notContainsText" dxfId="4" priority="18" stopIfTrue="1" operator="notContains" text="EUR">
+    <cfRule type="notContainsText" dxfId="19" priority="34" stopIfTrue="1" operator="notContains" text="EUR">
       <formula>ISERROR(SEARCH("EUR",D2))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="3" priority="18">
+    <cfRule type="containsBlanks" dxfId="18" priority="34">
       <formula>LEN(TRIM(D2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G23">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Vendita">
+    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="Vendita">
       <formula>NOT(ISERROR(SEARCH("Vendita",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Acquisto">
+    <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="Acquisto">
       <formula>NOT(ISERROR(SEARCH("Acquisto",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations disablePrompts="1" count="1">
+  <conditionalFormatting sqref="J2:J23">
+    <cfRule type="containsText" dxfId="9" priority="1" operator="containsText" text="NEW">
+      <formula>NOT(ISERROR(SEARCH("NEW",J2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="2" operator="containsText" text="Multi-Asset">
+      <formula>NOT(ISERROR(SEARCH("Multi-Asset",J2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="3" operator="containsText" text="Altro">
+      <formula>NOT(ISERROR(SEARCH("Altro",J2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="4" operator="containsText" text="Obbligazionario">
+      <formula>NOT(ISERROR(SEARCH("Obbligazionario",J2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="Obblig.">
+      <formula>NOT(ISERROR(SEARCH("Obblig.",J2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="ETF">
+      <formula>NOT(ISERROR(SEARCH("ETF",J2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="7" operator="containsText" text="Azionario">
+      <formula>NOT(ISERROR(SEARCH("Azionario",J2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="8" operator="containsText" text="Liquidità">
+      <formula>NOT(ISERROR(SEARCH("Liquidità",J2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="9" operator="containsText" text="Bilanciato">
+      <formula>NOT(ISERROR(SEARCH("Bilanciato",J2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="10" operator="containsText" text="Certif">
+      <formula>NOT(ISERROR(SEARCH("Certif",J2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G23" xr:uid="{786B1B08-543B-41BE-8266-499A04655516}">
       <formula1>"Acquisto,Vendita,-"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Release V1.0: Cleanup and Documentation Update
</commit_message>
<xml_diff>
--- a/0. Dati Iniziali/PortfolioMP_Acquisti.xlsx
+++ b/0. Dati Iniziali/PortfolioMP_Acquisti.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\PerixMonitor\0. Dati Iniziali\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6FC9E3-1146-40EF-AB33-217849B2528A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1023EFCE-2E88-4B2E-825A-D3D08ED78F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="490" windowWidth="38620" windowHeight="21220" xr2:uid="{461EA0C3-CC98-4DCD-BC5C-C997A9959903}"/>
   </bookViews>
@@ -435,7 +435,6 @@
   <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -460,16 +459,13 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -482,11 +478,15 @@
     <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="31">
     <dxf>
       <fill>
         <patternFill>
@@ -563,48 +563,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFEB8953"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -663,6 +621,15 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <color auto="1"/>
@@ -700,51 +667,40 @@
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor indexed="65"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
         <top style="thin">
           <color indexed="64"/>
         </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="12" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
       </border>
     </dxf>
     <dxf>
@@ -795,14 +751,14 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
           <bgColor auto="1"/>
         </patternFill>
       </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -848,7 +804,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="4" formatCode="#,##0.00"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -868,12 +824,6 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -999,24 +949,24 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{04F4BF02-F5A0-427F-92C4-A60283CF04F1}" name="Table1" displayName="Table1" ref="A1:K23" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35" tableBorderDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{04F4BF02-F5A0-427F-92C4-A60283CF04F1}" name="Table1" displayName="Table1" ref="A1:K23" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29" tableBorderDxfId="28">
   <autoFilter ref="A1:K23" xr:uid="{04F4BF02-F5A0-427F-92C4-A60283CF04F1}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B8061C36-8993-4203-ABD6-C7BF7558D40C}" name="Descrizione Titolo" dataDxfId="33"/>
-    <tableColumn id="2" xr3:uid="{C4CDF0AD-2602-44A7-AA26-292542A274A0}" name="ISIN" dataDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{0A18EC50-C250-41F4-83C1-E84B3FDD76A5}" name="Quantità" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{F21CA34D-52E3-4C7A-A959-24C01F694687}" name="Divisa" dataDxfId="30"/>
-    <tableColumn id="5" xr3:uid="{5C9AD5B2-888B-43C8-AC2C-1789ADAB0AD8}" name="Prezzo Carico (EUR)" dataDxfId="29"/>
-    <tableColumn id="6" xr3:uid="{1CC3BD49-EF04-4684-84DC-5AB42F08A1CD}" name="Data (acquisto/vendita)" dataDxfId="28"/>
-    <tableColumn id="7" xr3:uid="{0B72A75D-196B-42C0-9E49-163198DF8CDB}" name="Operazione" dataDxfId="27"/>
-    <tableColumn id="8" xr3:uid="{8C52C664-8EA8-4E89-892F-C9CCC6BB2E54}" name="Prezzo Operazione (EUR)" dataDxfId="26">
+    <tableColumn id="1" xr3:uid="{B8061C36-8993-4203-ABD6-C7BF7558D40C}" name="Descrizione Titolo" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{C4CDF0AD-2602-44A7-AA26-292542A274A0}" name="ISIN" dataDxfId="26"/>
+    <tableColumn id="3" xr3:uid="{0A18EC50-C250-41F4-83C1-E84B3FDD76A5}" name="Quantità" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{F21CA34D-52E3-4C7A-A959-24C01F694687}" name="Divisa" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{5C9AD5B2-888B-43C8-AC2C-1789ADAB0AD8}" name="Prezzo Carico (EUR)" dataDxfId="23"/>
+    <tableColumn id="6" xr3:uid="{1CC3BD49-EF04-4684-84DC-5AB42F08A1CD}" name="Data (acquisto/vendita)" dataDxfId="22"/>
+    <tableColumn id="7" xr3:uid="{0B72A75D-196B-42C0-9E49-163198DF8CDB}" name="Operazione" dataDxfId="21"/>
+    <tableColumn id="8" xr3:uid="{8C52C664-8EA8-4E89-892F-C9CCC6BB2E54}" name="Prezzo Operazione (EUR)" dataDxfId="20">
       <calculatedColumnFormula>+Table1[[#This Row],[Prezzo Carico (EUR)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{20AB3F10-3CEF-4BB7-ACA8-F58F613D5EBF}" name="Prezzo Corrente (EUR)" dataDxfId="25">
+    <tableColumn id="9" xr3:uid="{20AB3F10-3CEF-4BB7-ACA8-F58F613D5EBF}" name="Prezzo Corrente (EUR)" dataDxfId="19">
       <calculatedColumnFormula>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{8B0704F8-8C2E-42BE-A30C-03EF7C2730A1}" name="Tipologia" dataDxfId="23"/>
-    <tableColumn id="10" xr3:uid="{7F8241B6-2FCB-4564-8F24-4D4146A82E8B}" name="Controvalore (EUR)" dataDxfId="24">
+    <tableColumn id="11" xr3:uid="{8B0704F8-8C2E-42BE-A30C-03EF7C2730A1}" name="Tipologia" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{7F8241B6-2FCB-4564-8F24-4D4146A82E8B}" name="Controvalore (EUR)" dataDxfId="17">
       <calculatedColumnFormula>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1345,7 +1295,7 @@
   <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+      <selection activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1362,906 +1312,910 @@
     <col min="10" max="10" width="24.54296875" customWidth="1"/>
     <col min="11" max="11" width="21.26953125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6.7265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.08984375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.08984375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="9.08984375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="5.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="9" t="s">
+      <c r="J1" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="K1" s="15" t="s">
         <v>56</v>
+      </c>
+      <c r="O1" s="16">
+        <f>SUM(Table1[Controvalore (EUR)])</f>
+        <v>477085.93007820012</v>
       </c>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2" s="21">
         <v>200</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="23">
         <v>91.314800000000005</v>
       </c>
-      <c r="F2" s="12">
+      <c r="F2" s="11">
         <v>45002</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="4">
+      <c r="H2" s="21">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>91.314800000000005</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="21">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>91.314800000000005</v>
       </c>
-      <c r="J2" s="24" t="s">
+      <c r="J2" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="K2" s="20">
+      <c r="K2" s="24">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>18262.960000000003</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="21">
         <v>250</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="23">
         <v>90.38</v>
       </c>
-      <c r="F3" s="12">
+      <c r="F3" s="11">
         <v>45002</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="4">
+      <c r="H3" s="21">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>90.38</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="21">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>90.38</v>
       </c>
-      <c r="J3" s="24" t="s">
+      <c r="J3" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="K3" s="20">
+      <c r="K3" s="24">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>22595</v>
       </c>
-      <c r="O3" s="21">
+      <c r="O3" s="17">
         <v>-22708.055199999999</v>
       </c>
-      <c r="P3" s="22">
+      <c r="P3" s="18">
         <v>45355</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="21">
         <v>786.29</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="21">
         <v>28.88</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="11">
         <v>45355</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="G4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="4">
+      <c r="H4" s="21">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>28.88</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="21">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>28.88</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="J4" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="K4" s="20">
+      <c r="K4" s="24">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>22708.055199999999</v>
       </c>
-      <c r="N4" s="4">
+      <c r="N4" s="3">
         <v>32.729999999999997</v>
       </c>
-      <c r="O4" s="4">
+      <c r="O4" s="3">
         <f>+C4*N4</f>
         <v>25735.271699999998</v>
       </c>
-      <c r="P4" s="12">
+      <c r="P4" s="11">
         <f ca="1">TODAY()</f>
-        <v>46049</v>
-      </c>
-      <c r="Q4" s="4">
+        <v>46052</v>
+      </c>
+      <c r="Q4" s="3">
         <f>+O4-K4</f>
         <v>3027.2164999999986</v>
       </c>
-      <c r="S4" s="23">
+      <c r="S4" s="19">
         <f ca="1">XIRR(O3:O4,P3:P4)</f>
-        <v>6.8031427264213559E-2</v>
+        <v>6.7728909850120561E-2</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="21">
         <v>808.88599999999997</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="21">
         <v>117.33</v>
       </c>
-      <c r="F5" s="12">
+      <c r="F5" s="11">
         <v>45355</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="4">
+      <c r="H5" s="21">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>117.33</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="21">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>117.33</v>
       </c>
-      <c r="J5" s="24" t="s">
+      <c r="J5" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="K5" s="20">
+      <c r="K5" s="24">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>94906.594379999995</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="21">
         <v>255.42699999999999</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="21">
         <v>242.5</v>
       </c>
-      <c r="F6" s="12">
+      <c r="F6" s="11">
         <v>45355</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="4">
+      <c r="H6" s="21">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>242.5</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="21">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>242.5</v>
       </c>
-      <c r="J6" s="24" t="s">
+      <c r="J6" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="K6" s="20">
+      <c r="K6" s="24">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>61941.047500000001</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="21">
         <v>570</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="23">
         <v>8.8187540000000002</v>
       </c>
-      <c r="F7" s="12">
+      <c r="F7" s="11">
         <v>45702</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="G7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="21">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>8.8187540000000002</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="21">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>8.8187540000000002</v>
       </c>
-      <c r="J7" s="24" t="s">
+      <c r="J7" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="K7" s="20">
+      <c r="K7" s="24">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>5026.6897799999997</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="21">
         <v>47</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="21">
         <v>108.097021</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="11">
         <v>45705</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="4">
+      <c r="H8" s="21">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>108.097021</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="21">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>108.097021</v>
       </c>
-      <c r="J8" s="24" t="s">
+      <c r="J8" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="K8" s="20">
+      <c r="K8" s="24">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>5080.5599869999996</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="21">
         <v>945.54899999999998</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="D9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="21">
         <v>16.910799999999998</v>
       </c>
-      <c r="F9" s="12">
+      <c r="F9" s="11">
         <v>45702</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="21">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>16.910799999999998</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="21">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>16.910799999999998</v>
       </c>
-      <c r="J9" s="24" t="s">
+      <c r="J9" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="K9" s="20">
+      <c r="K9" s="24">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>15989.990029199998</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="21">
         <v>3198</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="21">
         <v>5</v>
       </c>
-      <c r="F10" s="12">
+      <c r="F10" s="11">
         <v>45702</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="4">
+      <c r="H10" s="21">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>5</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="21">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>5</v>
       </c>
-      <c r="J10" s="24" t="s">
+      <c r="J10" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="K10" s="20">
+      <c r="K10" s="24">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>15990</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="21">
         <v>104.37</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="21">
         <v>198.97</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="11">
         <v>45355</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="21">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>198.97</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="21">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>198.97</v>
       </c>
-      <c r="J11" s="24" t="s">
+      <c r="J11" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="K11" s="20">
+      <c r="K11" s="24">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>20766.498900000002</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="21">
         <v>207.953</v>
       </c>
-      <c r="D12" s="11" t="s">
+      <c r="D12" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="21">
         <v>117.95</v>
       </c>
-      <c r="F12" s="12">
+      <c r="F12" s="11">
         <v>45355</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="G12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="4">
+      <c r="H12" s="21">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>117.95</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="21">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>117.95</v>
       </c>
-      <c r="J12" s="24" t="s">
+      <c r="J12" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="K12" s="20">
+      <c r="K12" s="24">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>24528.056350000003</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="21">
         <v>448.18400000000003</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="21">
         <v>32.000999999999998</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="11">
         <v>45355</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="G13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="21">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>32.000999999999998</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="21">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>32.000999999999998</v>
       </c>
-      <c r="J13" s="24" t="s">
+      <c r="J13" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="K13" s="20">
+      <c r="K13" s="24">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>14342.336184</v>
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="21">
         <v>117.944</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="21">
         <v>188.5</v>
       </c>
-      <c r="F14" s="12">
+      <c r="F14" s="11">
         <v>45806</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="G14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H14" s="21">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>188.5</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="21">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>188.5</v>
       </c>
-      <c r="J14" s="24" t="s">
+      <c r="J14" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="K14" s="20">
+      <c r="K14" s="24">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>22232.444</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A15" s="10" t="s">
+      <c r="A15" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="21">
         <v>290.43</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="21">
         <v>83.850999999999999</v>
       </c>
-      <c r="F15" s="12">
+      <c r="F15" s="11">
         <v>45355</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="4">
+      <c r="H15" s="21">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>83.850999999999999</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="21">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>83.850999999999999</v>
       </c>
-      <c r="J15" s="24" t="s">
+      <c r="J15" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="K15" s="20">
+      <c r="K15" s="24">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>24352.845929999999</v>
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A16" s="10" t="s">
+      <c r="A16" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="21">
         <v>586.02</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="21">
         <v>19.100000000000001</v>
       </c>
-      <c r="F16" s="12">
+      <c r="F16" s="11">
         <v>45355</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="G16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="21">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>19.100000000000001</v>
       </c>
-      <c r="I16" s="4">
+      <c r="I16" s="21">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>19.100000000000001</v>
       </c>
-      <c r="J16" s="24" t="s">
+      <c r="J16" s="20" t="s">
         <v>58</v>
       </c>
-      <c r="K16" s="20">
+      <c r="K16" s="24">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>11192.982</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="21">
         <v>86</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="21">
         <v>93.194999999999993</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="11">
         <v>45706</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="G17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H17" s="4">
+      <c r="H17" s="21">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>93.194999999999993</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17" s="21">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>93.194999999999993</v>
       </c>
-      <c r="J17" s="24" t="s">
+      <c r="J17" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="K17" s="20">
+      <c r="K17" s="24">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>8014.7699999999995</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A18" s="10" t="s">
+      <c r="A18" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="21">
         <v>99.85</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="D18" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="21">
         <v>100</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F18" s="11">
         <v>45701</v>
       </c>
-      <c r="G18" s="3" t="s">
+      <c r="G18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H18" s="4">
+      <c r="H18" s="21">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>100</v>
       </c>
-      <c r="I18" s="4">
+      <c r="I18" s="21">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>100</v>
       </c>
-      <c r="J18" s="24" t="s">
+      <c r="J18" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="K18" s="20">
+      <c r="K18" s="24">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>9985</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="21">
         <v>200</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D19" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="21">
         <v>97.14</v>
       </c>
-      <c r="F19" s="12">
+      <c r="F19" s="11">
         <v>45355</v>
       </c>
-      <c r="G19" s="3" t="s">
+      <c r="G19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H19" s="4">
+      <c r="H19" s="21">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>97.14</v>
       </c>
-      <c r="I19" s="4">
+      <c r="I19" s="21">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>97.14</v>
       </c>
-      <c r="J19" s="24" t="s">
+      <c r="J19" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="K19" s="20">
+      <c r="K19" s="24">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>19428</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="15">
+      <c r="C20" s="22">
         <v>155</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D20" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="21">
         <v>94.621290000000002</v>
       </c>
-      <c r="F20" s="17">
+      <c r="F20" s="14">
         <v>46044</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H20" s="18">
+      <c r="H20" s="22">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>94.621290000000002</v>
       </c>
-      <c r="I20" s="18">
+      <c r="I20" s="22">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>94.621290000000002</v>
       </c>
-      <c r="J20" s="24" t="s">
+      <c r="J20" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="K20" s="20">
+      <c r="K20" s="24">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>14666.299950000001</v>
       </c>
       <c r="O20" s="1"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A21" s="14" t="s">
+      <c r="A21" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="15">
-        <v>2387</v>
-      </c>
-      <c r="D21" s="16" t="s">
+      <c r="C21" s="22">
+        <v>237</v>
+      </c>
+      <c r="D21" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="21">
         <v>42.381138999999997</v>
       </c>
-      <c r="F21" s="17">
+      <c r="F21" s="14">
         <v>46044</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H21" s="18">
+      <c r="H21" s="22">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>42.381138999999997</v>
       </c>
-      <c r="I21" s="18">
+      <c r="I21" s="22">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>42.381138999999997</v>
       </c>
-      <c r="J21" s="24" t="s">
+      <c r="J21" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="K21" s="20">
+      <c r="K21" s="24">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
-        <v>101163.77879299999</v>
+        <v>10044.329942999999</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="21">
         <v>15</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="21">
         <v>1009.464666</v>
       </c>
-      <c r="F22" s="12">
+      <c r="F22" s="11">
         <v>46048</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H22" s="4">
+      <c r="H22" s="21">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>1009.464666</v>
       </c>
-      <c r="I22" s="4">
+      <c r="I22" s="21">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>1009.464666</v>
       </c>
-      <c r="J22" s="24" t="s">
+      <c r="J22" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="K22" s="20">
+      <c r="K22" s="24">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>15141.96999</v>
       </c>
       <c r="O22" s="1"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A23" s="14" t="s">
+      <c r="A23" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="15">
+      <c r="C23" s="22">
         <v>205</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="21">
         <v>97.021951000000001</v>
       </c>
-      <c r="F23" s="17">
+      <c r="F23" s="14">
         <v>46044</v>
       </c>
-      <c r="G23" s="3" t="s">
+      <c r="G23" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H23" s="18">
+      <c r="H23" s="22">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>97.021951000000001</v>
       </c>
-      <c r="I23" s="18">
+      <c r="I23" s="22">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>97.021951000000001</v>
       </c>
-      <c r="J23" s="24" t="s">
+      <c r="J23" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="K23" s="20">
+      <c r="K23" s="24">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>19889.499954999999</v>
       </c>
@@ -2269,31 +2223,31 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:A23">
-    <cfRule type="containsText" dxfId="22" priority="32" stopIfTrue="1" operator="containsText" text="BTP">
+    <cfRule type="containsText" dxfId="16" priority="32" stopIfTrue="1" operator="containsText" text="BTP">
       <formula>NOT(ISERROR(SEARCH("BTP",A2)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="21" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="33" stopIfTrue="1">
       <formula>IF(AND(ISNUMBER(SEARCH("H2O", A2)), ISNUMBER(SEARCH("SP", A2))), 1,0)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C23">
-    <cfRule type="containsBlanks" dxfId="20" priority="30">
+    <cfRule type="containsBlanks" dxfId="14" priority="30">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D23">
-    <cfRule type="notContainsText" dxfId="19" priority="34" stopIfTrue="1" operator="notContains" text="EUR">
+    <cfRule type="notContainsText" dxfId="13" priority="34" stopIfTrue="1" operator="notContains" text="EUR">
       <formula>ISERROR(SEARCH("EUR",D2))</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="18" priority="34">
+    <cfRule type="containsBlanks" dxfId="12" priority="34">
       <formula>LEN(TRIM(D2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G23">
-    <cfRule type="containsText" dxfId="17" priority="17" operator="containsText" text="Vendita">
+    <cfRule type="containsText" dxfId="11" priority="17" operator="containsText" text="Vendita">
       <formula>NOT(ISERROR(SEARCH("Vendita",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="18" operator="containsText" text="Acquisto">
+    <cfRule type="containsText" dxfId="10" priority="18" operator="containsText" text="Acquisto">
       <formula>NOT(ISERROR(SEARCH("Acquisto",G2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Refactor Ingestion Logic (Transaction-Only), Persistence of UI Selection, Doc Update
</commit_message>
<xml_diff>
--- a/0. Dati Iniziali/PortfolioMP_Acquisti.xlsx
+++ b/0. Dati Iniziali/PortfolioMP_Acquisti.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29725"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\PerixMonitor\0. Dati Iniziali\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1023EFCE-2E88-4B2E-825A-D3D08ED78F3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C560FD3-255B-4118-8203-1E085C7D8AF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="490" windowWidth="38620" windowHeight="21220" xr2:uid="{461EA0C3-CC98-4DCD-BC5C-C997A9959903}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="32830" windowHeight="21000" xr2:uid="{461EA0C3-CC98-4DCD-BC5C-C997A9959903}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -275,7 +275,7 @@
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="164" formatCode="#,##0.00;;\-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,6 +307,14 @@
     <font>
       <b/>
       <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -469,7 +477,6 @@
     <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="8" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -482,6 +489,7 @@
     <xf numFmtId="4" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="8" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1295,7 +1303,7 @@
   <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1352,7 +1360,7 @@
       <c r="K1" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="O1" s="16">
+      <c r="O1" s="24">
         <f>SUM(Table1[Controvalore (EUR)])</f>
         <v>477085.93007820012</v>
       </c>
@@ -1364,13 +1372,13 @@
       <c r="B2" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C2" s="20">
         <v>200</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="23">
+      <c r="E2" s="22">
         <v>91.314800000000005</v>
       </c>
       <c r="F2" s="11">
@@ -1379,18 +1387,18 @@
       <c r="G2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="21">
+      <c r="H2" s="20">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>91.314800000000005</v>
       </c>
-      <c r="I2" s="21">
+      <c r="I2" s="20">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>91.314800000000005</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="K2" s="24">
+      <c r="K2" s="23">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>18262.960000000003</v>
       </c>
@@ -1402,13 +1410,13 @@
       <c r="B3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="20">
         <v>250</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="23">
+      <c r="E3" s="22">
         <v>90.38</v>
       </c>
       <c r="F3" s="11">
@@ -1417,25 +1425,25 @@
       <c r="G3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="21">
+      <c r="H3" s="20">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>90.38</v>
       </c>
-      <c r="I3" s="21">
+      <c r="I3" s="20">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>90.38</v>
       </c>
-      <c r="J3" s="20" t="s">
+      <c r="J3" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="K3" s="24">
+      <c r="K3" s="23">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>22595</v>
       </c>
-      <c r="O3" s="17">
+      <c r="O3" s="16">
         <v>-22708.055199999999</v>
       </c>
-      <c r="P3" s="18">
+      <c r="P3" s="17">
         <v>45355</v>
       </c>
     </row>
@@ -1446,13 +1454,13 @@
       <c r="B4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C4" s="20">
         <v>786.29</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="20">
         <v>28.88</v>
       </c>
       <c r="F4" s="11">
@@ -1461,18 +1469,18 @@
       <c r="G4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="21">
+      <c r="H4" s="20">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>28.88</v>
       </c>
-      <c r="I4" s="21">
+      <c r="I4" s="20">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>28.88</v>
       </c>
-      <c r="J4" s="20" t="s">
+      <c r="J4" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="K4" s="24">
+      <c r="K4" s="23">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>22708.055199999999</v>
       </c>
@@ -1485,15 +1493,15 @@
       </c>
       <c r="P4" s="11">
         <f ca="1">TODAY()</f>
-        <v>46052</v>
+        <v>46053</v>
       </c>
       <c r="Q4" s="3">
         <f>+O4-K4</f>
         <v>3027.2164999999986</v>
       </c>
-      <c r="S4" s="19">
+      <c r="S4" s="18">
         <f ca="1">XIRR(O3:O4,P3:P4)</f>
-        <v>6.7728909850120561E-2</v>
+        <v>6.7628666758537292E-2</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
@@ -1503,13 +1511,13 @@
       <c r="B5" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C5" s="20">
         <v>808.88599999999997</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="20">
         <v>117.33</v>
       </c>
       <c r="F5" s="11">
@@ -1518,18 +1526,18 @@
       <c r="G5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="21">
+      <c r="H5" s="20">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>117.33</v>
       </c>
-      <c r="I5" s="21">
+      <c r="I5" s="20">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>117.33</v>
       </c>
-      <c r="J5" s="20" t="s">
+      <c r="J5" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="K5" s="24">
+      <c r="K5" s="23">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>94906.594379999995</v>
       </c>
@@ -1541,13 +1549,13 @@
       <c r="B6" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C6" s="20">
         <v>255.42699999999999</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="20">
         <v>242.5</v>
       </c>
       <c r="F6" s="11">
@@ -1556,18 +1564,18 @@
       <c r="G6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="21">
+      <c r="H6" s="20">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>242.5</v>
       </c>
-      <c r="I6" s="21">
+      <c r="I6" s="20">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>242.5</v>
       </c>
-      <c r="J6" s="20" t="s">
+      <c r="J6" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="K6" s="24">
+      <c r="K6" s="23">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>61941.047500000001</v>
       </c>
@@ -1579,13 +1587,13 @@
       <c r="B7" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C7" s="20">
         <v>570</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="22">
         <v>8.8187540000000002</v>
       </c>
       <c r="F7" s="11">
@@ -1594,18 +1602,18 @@
       <c r="G7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="21">
+      <c r="H7" s="20">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>8.8187540000000002</v>
       </c>
-      <c r="I7" s="21">
+      <c r="I7" s="20">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>8.8187540000000002</v>
       </c>
-      <c r="J7" s="20" t="s">
+      <c r="J7" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="K7" s="24">
+      <c r="K7" s="23">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>5026.6897799999997</v>
       </c>
@@ -1617,13 +1625,13 @@
       <c r="B8" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C8" s="20">
         <v>47</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="20">
         <v>108.097021</v>
       </c>
       <c r="F8" s="11">
@@ -1632,18 +1640,18 @@
       <c r="G8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="21">
+      <c r="H8" s="20">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>108.097021</v>
       </c>
-      <c r="I8" s="21">
+      <c r="I8" s="20">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>108.097021</v>
       </c>
-      <c r="J8" s="20" t="s">
+      <c r="J8" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="K8" s="24">
+      <c r="K8" s="23">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>5080.5599869999996</v>
       </c>
@@ -1655,13 +1663,13 @@
       <c r="B9" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C9" s="20">
         <v>945.54899999999998</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="20">
         <v>16.910799999999998</v>
       </c>
       <c r="F9" s="11">
@@ -1670,18 +1678,18 @@
       <c r="G9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="21">
+      <c r="H9" s="20">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>16.910799999999998</v>
       </c>
-      <c r="I9" s="21">
+      <c r="I9" s="20">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>16.910799999999998</v>
       </c>
-      <c r="J9" s="20" t="s">
+      <c r="J9" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="K9" s="24">
+      <c r="K9" s="23">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>15989.990029199998</v>
       </c>
@@ -1693,13 +1701,13 @@
       <c r="B10" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C10" s="20">
         <v>3198</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="20">
         <v>5</v>
       </c>
       <c r="F10" s="11">
@@ -1708,18 +1716,18 @@
       <c r="G10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="21">
+      <c r="H10" s="20">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>5</v>
       </c>
-      <c r="I10" s="21">
+      <c r="I10" s="20">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>5</v>
       </c>
-      <c r="J10" s="20" t="s">
+      <c r="J10" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="K10" s="24">
+      <c r="K10" s="23">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>15990</v>
       </c>
@@ -1731,13 +1739,13 @@
       <c r="B11" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C11" s="20">
         <v>104.37</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="20">
         <v>198.97</v>
       </c>
       <c r="F11" s="11">
@@ -1746,18 +1754,18 @@
       <c r="G11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="21">
+      <c r="H11" s="20">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>198.97</v>
       </c>
-      <c r="I11" s="21">
+      <c r="I11" s="20">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>198.97</v>
       </c>
-      <c r="J11" s="20" t="s">
+      <c r="J11" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="K11" s="24">
+      <c r="K11" s="23">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>20766.498900000002</v>
       </c>
@@ -1769,13 +1777,13 @@
       <c r="B12" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="21">
+      <c r="C12" s="20">
         <v>207.953</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="20">
         <v>117.95</v>
       </c>
       <c r="F12" s="11">
@@ -1784,18 +1792,18 @@
       <c r="G12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="21">
+      <c r="H12" s="20">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>117.95</v>
       </c>
-      <c r="I12" s="21">
+      <c r="I12" s="20">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>117.95</v>
       </c>
-      <c r="J12" s="20" t="s">
+      <c r="J12" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="K12" s="24">
+      <c r="K12" s="23">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>24528.056350000003</v>
       </c>
@@ -1807,13 +1815,13 @@
       <c r="B13" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C13" s="20">
         <v>448.18400000000003</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E13" s="21">
+      <c r="E13" s="20">
         <v>32.000999999999998</v>
       </c>
       <c r="F13" s="11">
@@ -1822,18 +1830,18 @@
       <c r="G13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H13" s="21">
+      <c r="H13" s="20">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>32.000999999999998</v>
       </c>
-      <c r="I13" s="21">
+      <c r="I13" s="20">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>32.000999999999998</v>
       </c>
-      <c r="J13" s="20" t="s">
+      <c r="J13" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="K13" s="24">
+      <c r="K13" s="23">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>14342.336184</v>
       </c>
@@ -1845,13 +1853,13 @@
       <c r="B14" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="21">
+      <c r="C14" s="20">
         <v>117.944</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E14" s="21">
+      <c r="E14" s="20">
         <v>188.5</v>
       </c>
       <c r="F14" s="11">
@@ -1860,18 +1868,18 @@
       <c r="G14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H14" s="21">
+      <c r="H14" s="20">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>188.5</v>
       </c>
-      <c r="I14" s="21">
+      <c r="I14" s="20">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>188.5</v>
       </c>
-      <c r="J14" s="20" t="s">
+      <c r="J14" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="K14" s="24">
+      <c r="K14" s="23">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>22232.444</v>
       </c>
@@ -1883,13 +1891,13 @@
       <c r="B15" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C15" s="21">
+      <c r="C15" s="20">
         <v>290.43</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E15" s="21">
+      <c r="E15" s="20">
         <v>83.850999999999999</v>
       </c>
       <c r="F15" s="11">
@@ -1898,18 +1906,18 @@
       <c r="G15" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="21">
+      <c r="H15" s="20">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>83.850999999999999</v>
       </c>
-      <c r="I15" s="21">
+      <c r="I15" s="20">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>83.850999999999999</v>
       </c>
-      <c r="J15" s="20" t="s">
+      <c r="J15" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="K15" s="24">
+      <c r="K15" s="23">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>24352.845929999999</v>
       </c>
@@ -1921,13 +1929,13 @@
       <c r="B16" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="21">
+      <c r="C16" s="20">
         <v>586.02</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E16" s="21">
+      <c r="E16" s="20">
         <v>19.100000000000001</v>
       </c>
       <c r="F16" s="11">
@@ -1936,18 +1944,18 @@
       <c r="G16" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H16" s="21">
+      <c r="H16" s="20">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>19.100000000000001</v>
       </c>
-      <c r="I16" s="21">
+      <c r="I16" s="20">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>19.100000000000001</v>
       </c>
-      <c r="J16" s="20" t="s">
+      <c r="J16" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="K16" s="24">
+      <c r="K16" s="23">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>11192.982</v>
       </c>
@@ -1959,13 +1967,13 @@
       <c r="B17" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="C17" s="21">
+      <c r="C17" s="20">
         <v>86</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="21">
+      <c r="E17" s="20">
         <v>93.194999999999993</v>
       </c>
       <c r="F17" s="11">
@@ -1974,18 +1982,18 @@
       <c r="G17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H17" s="21">
+      <c r="H17" s="20">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>93.194999999999993</v>
       </c>
-      <c r="I17" s="21">
+      <c r="I17" s="20">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>93.194999999999993</v>
       </c>
-      <c r="J17" s="20" t="s">
+      <c r="J17" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="K17" s="24">
+      <c r="K17" s="23">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>8014.7699999999995</v>
       </c>
@@ -1997,13 +2005,13 @@
       <c r="B18" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="C18" s="21">
+      <c r="C18" s="20">
         <v>99.85</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="21">
+      <c r="E18" s="20">
         <v>100</v>
       </c>
       <c r="F18" s="11">
@@ -2012,18 +2020,18 @@
       <c r="G18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H18" s="21">
+      <c r="H18" s="20">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>100</v>
       </c>
-      <c r="I18" s="21">
+      <c r="I18" s="20">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>100</v>
       </c>
-      <c r="J18" s="20" t="s">
+      <c r="J18" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="K18" s="24">
+      <c r="K18" s="23">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>9985</v>
       </c>
@@ -2035,13 +2043,13 @@
       <c r="B19" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C19" s="21">
+      <c r="C19" s="20">
         <v>200</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E19" s="21">
+      <c r="E19" s="20">
         <v>97.14</v>
       </c>
       <c r="F19" s="11">
@@ -2050,18 +2058,18 @@
       <c r="G19" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H19" s="21">
+      <c r="H19" s="20">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>97.14</v>
       </c>
-      <c r="I19" s="21">
+      <c r="I19" s="20">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>97.14</v>
       </c>
-      <c r="J19" s="20" t="s">
+      <c r="J19" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="K19" s="24">
+      <c r="K19" s="23">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>19428</v>
       </c>
@@ -2073,13 +2081,13 @@
       <c r="B20" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="22">
+      <c r="C20" s="21">
         <v>155</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E20" s="21">
+      <c r="E20" s="20">
         <v>94.621290000000002</v>
       </c>
       <c r="F20" s="14">
@@ -2088,18 +2096,18 @@
       <c r="G20" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H20" s="22">
+      <c r="H20" s="21">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>94.621290000000002</v>
       </c>
-      <c r="I20" s="22">
+      <c r="I20" s="21">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>94.621290000000002</v>
       </c>
-      <c r="J20" s="20" t="s">
+      <c r="J20" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="K20" s="24">
+      <c r="K20" s="23">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>14666.299950000001</v>
       </c>
@@ -2112,13 +2120,13 @@
       <c r="B21" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="22">
+      <c r="C21" s="21">
         <v>237</v>
       </c>
       <c r="D21" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="21">
+      <c r="E21" s="20">
         <v>42.381138999999997</v>
       </c>
       <c r="F21" s="14">
@@ -2127,18 +2135,18 @@
       <c r="G21" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H21" s="22">
+      <c r="H21" s="21">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>42.381138999999997</v>
       </c>
-      <c r="I21" s="22">
+      <c r="I21" s="21">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>42.381138999999997</v>
       </c>
-      <c r="J21" s="20" t="s">
+      <c r="J21" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="K21" s="24">
+      <c r="K21" s="23">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>10044.329942999999</v>
       </c>
@@ -2150,13 +2158,13 @@
       <c r="B22" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="21">
+      <c r="C22" s="20">
         <v>15</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="21">
+      <c r="E22" s="20">
         <v>1009.464666</v>
       </c>
       <c r="F22" s="11">
@@ -2165,18 +2173,18 @@
       <c r="G22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H22" s="21">
+      <c r="H22" s="20">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>1009.464666</v>
       </c>
-      <c r="I22" s="21">
+      <c r="I22" s="20">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>1009.464666</v>
       </c>
-      <c r="J22" s="20" t="s">
+      <c r="J22" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="K22" s="24">
+      <c r="K22" s="23">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>15141.96999</v>
       </c>
@@ -2189,13 +2197,13 @@
       <c r="B23" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="22">
+      <c r="C23" s="21">
         <v>205</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E23" s="21">
+      <c r="E23" s="20">
         <v>97.021951000000001</v>
       </c>
       <c r="F23" s="14">
@@ -2204,18 +2212,18 @@
       <c r="G23" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="H23" s="22">
+      <c r="H23" s="21">
         <f>+Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>97.021951000000001</v>
       </c>
-      <c r="I23" s="22">
+      <c r="I23" s="21">
         <f>+Table1[[#This Row],[Prezzo Operazione (EUR)]]</f>
         <v>97.021951000000001</v>
       </c>
-      <c r="J23" s="20" t="s">
+      <c r="J23" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="K23" s="24">
+      <c r="K23" s="23">
         <f>+Table1[[#This Row],[Quantità]]*Table1[[#This Row],[Prezzo Carico (EUR)]]</f>
         <v>19889.499954999999</v>
       </c>

</xml_diff>

<commit_message>
LLM Integration Fix: GPT-5, Native Search, CORS support, and UI refinements
</commit_message>
<xml_diff>
--- a/0. Dati Iniziali/PortfolioMP_Acquisti.xlsx
+++ b/0. Dati Iniziali/PortfolioMP_Acquisti.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\PerixMonitor\0. Dati Iniziali\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E84D969-71F3-42E9-A7B1-E47A4C36E73A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBF9D227-85C6-41E1-B4AD-4627F0880037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{461EA0C3-CC98-4DCD-BC5C-C997A9959903}"/>
+    <workbookView xWindow="8450" yWindow="1820" windowWidth="26270" windowHeight="10310" xr2:uid="{461EA0C3-CC98-4DCD-BC5C-C997A9959903}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1337,8 +1337,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:U23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1522,7 +1522,7 @@
       </c>
       <c r="R4" s="11">
         <f ca="1">TODAY()</f>
-        <v>46053</v>
+        <v>46054</v>
       </c>
       <c r="S4" s="3">
         <f>+Q4-K4</f>
@@ -1530,7 +1530,7 @@
       </c>
       <c r="U4" s="18">
         <f ca="1">XIRR(Q3:Q4,R3:R4)</f>
-        <v>-0.46743708029389386</v>
+        <v>-0.4669568307697774</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.35">

</xml_diff>